<commit_message>
Feat : lecture modify
</commit_message>
<xml_diff>
--- a/homework/0501_homework.xlsx
+++ b/homework/0501_homework.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpzps\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CnuStudy\homework\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7B44E58D-9BD2-49C5-9E45-E16CA7F37B30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{97E64772-925A-4DFB-8B54-BE8B5F53E2B4}"/>
+    <workbookView xWindow="38278" yWindow="-118" windowWidth="29036" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="59">
   <si>
     <t>a</t>
   </si>
@@ -165,24 +164,70 @@
   </si>
   <si>
     <t>s = 0a000</t>
+  </si>
+  <si>
+    <t>0a005</t>
+  </si>
+  <si>
+    <t>0a006</t>
+  </si>
+  <si>
+    <t>0a007</t>
+  </si>
+  <si>
+    <t>0a008</t>
+  </si>
+  <si>
+    <t>0a009</t>
+  </si>
+  <si>
+    <t>0a010</t>
+  </si>
+  <si>
+    <t>0a011</t>
+  </si>
+  <si>
+    <t>0a012</t>
+  </si>
+  <si>
+    <t>0a013</t>
+  </si>
+  <si>
+    <t>0a014</t>
+  </si>
+  <si>
+    <t>0a015</t>
+  </si>
+  <si>
+    <t>0a016</t>
+  </si>
+  <si>
+    <t>0a017</t>
+  </si>
+  <si>
+    <t>0a018</t>
+  </si>
+  <si>
+    <t>null</t>
+    <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,8 +235,15 @@
       <b/>
       <sz val="18"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -625,26 +677,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E245F4-EEED-4FEA-BC18-620301ACF3F4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A8:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Y18" sqref="Y18"/>
+    <sheetView tabSelected="1" topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17.05" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" customWidth="1"/>
-    <col min="3" max="10" width="9.140625" style="2"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" customWidth="1"/>
+    <col min="3" max="10" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="8" spans="1:16" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="27.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" ht="17.7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -694,7 +746,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" ht="17.7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" t="s">
         <v>24</v>
       </c>
@@ -711,7 +763,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -728,7 +780,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>27</v>
       </c>
@@ -745,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>28</v>
       </c>
@@ -765,7 +817,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -786,22 +838,22 @@
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="G20" s="1"/>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="K21" s="7"/>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="K24" s="2"/>
     </row>
-    <row r="25" spans="1:21" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" ht="27.5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="10" t="s">
         <v>42</v>
       </c>
       <c r="K25" s="2"/>
     </row>
-    <row r="26" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="17.7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -862,8 +914,11 @@
       <c r="T26" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="U26" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="17.7" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B27" t="s">
         <v>40</v>
       </c>
@@ -881,7 +936,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -914,7 +969,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -979,34 +1034,77 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>43</v>
       </c>
-      <c r="Q30" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="D30" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="I30" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="M30" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="N30" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="O30" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Q30" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="R30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S30" s="2" t="s">
-        <v>18</v>
+        <v>54</v>
+      </c>
+      <c r="S30" s="1" t="s">
+        <v>55</v>
       </c>
       <c r="T30" s="2" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>

</xml_diff>